<commit_message>
Update summary disjoint (windows,granularity).xlsx
</commit_message>
<xml_diff>
--- a/ForegroundJobScheduler/results/Nonoverlapping windows/summary disjoint (windows,granularity).xlsx
+++ b/ForegroundJobScheduler/results/Nonoverlapping windows/summary disjoint (windows,granularity).xlsx
@@ -19409,11 +19409,21 @@
       <c r="G594" t="n">
         <v>0.0</v>
       </c>
-      <c r="H594"/>
-      <c r="I594"/>
-      <c r="J594"/>
-      <c r="K594"/>
-      <c r="L594"/>
+      <c r="H594" t="n">
+        <v>0.38011850620757043</v>
+      </c>
+      <c r="I594" t="n">
+        <v>0.32156712638572876</v>
+      </c>
+      <c r="J594" t="n">
+        <v>0.9123407056321989</v>
+      </c>
+      <c r="K594" t="n">
+        <v>0.9706896551724138</v>
+      </c>
+      <c r="L594" t="n">
+        <v>0.6902010050251256</v>
+      </c>
     </row>
     <row r="595">
       <c r="A595" t="s">
@@ -19437,11 +19447,21 @@
       <c r="G595" t="n">
         <v>0.0</v>
       </c>
-      <c r="H595"/>
-      <c r="I595"/>
-      <c r="J595"/>
-      <c r="K595"/>
-      <c r="L595"/>
+      <c r="H595" t="n">
+        <v>0.3881853480056075</v>
+      </c>
+      <c r="I595" t="n">
+        <v>0.3270220117558246</v>
+      </c>
+      <c r="J595" t="n">
+        <v>0.9104111829870422</v>
+      </c>
+      <c r="K595" t="n">
+        <v>0.9716666666666667</v>
+      </c>
+      <c r="L595" t="n">
+        <v>0.6910691823899371</v>
+      </c>
     </row>
     <row r="596">
       <c r="A596" t="s">
@@ -19493,11 +19513,21 @@
       <c r="G597" t="n">
         <v>0.0</v>
       </c>
-      <c r="H597"/>
-      <c r="I597"/>
-      <c r="J597"/>
-      <c r="K597"/>
-      <c r="L597"/>
+      <c r="H597" t="n">
+        <v>0.49903290145720575</v>
+      </c>
+      <c r="I597" t="n">
+        <v>0.4126770350680919</v>
+      </c>
+      <c r="J597" t="n">
+        <v>0.8844243231580867</v>
+      </c>
+      <c r="K597" t="n">
+        <v>0.9351851851851852</v>
+      </c>
+      <c r="L597" t="n">
+        <v>0.6958841463414634</v>
+      </c>
     </row>
     <row r="598">
       <c r="A598" t="s">
@@ -19521,11 +19551,21 @@
       <c r="G598" t="n">
         <v>0.0</v>
       </c>
-      <c r="H598"/>
-      <c r="I598"/>
-      <c r="J598"/>
-      <c r="K598"/>
-      <c r="L598"/>
+      <c r="H598" t="n">
+        <v>0.5097779619182066</v>
+      </c>
+      <c r="I598" t="n">
+        <v>0.42104244144356545</v>
+      </c>
+      <c r="J598" t="n">
+        <v>0.8807567888857353</v>
+      </c>
+      <c r="K598" t="n">
+        <v>0.9321824907521579</v>
+      </c>
+      <c r="L598" t="n">
+        <v>0.6979412327108165</v>
+      </c>
     </row>
     <row r="599">
       <c r="A599" t="s">
@@ -19577,11 +19617,21 @@
       <c r="G600" t="n">
         <v>0.0</v>
       </c>
-      <c r="H600"/>
-      <c r="I600"/>
-      <c r="J600"/>
-      <c r="K600"/>
-      <c r="L600"/>
+      <c r="H600" t="n">
+        <v>0.5213826062484477</v>
+      </c>
+      <c r="I600" t="n">
+        <v>0.41821880756241503</v>
+      </c>
+      <c r="J600" t="n">
+        <v>0.5861423656810953</v>
+      </c>
+      <c r="K600" t="n">
+        <v>0.6986374565856265</v>
+      </c>
+      <c r="L600" t="n">
+        <v>0.7742415928509838</v>
+      </c>
     </row>
     <row r="601">
       <c r="A601" t="s">
@@ -19605,11 +19655,21 @@
       <c r="G601" t="n">
         <v>0.0</v>
       </c>
-      <c r="H601"/>
-      <c r="I601"/>
-      <c r="J601"/>
-      <c r="K601"/>
-      <c r="L601"/>
+      <c r="H601" t="n">
+        <v>0.48637309446461324</v>
+      </c>
+      <c r="I601" t="n">
+        <v>0.38869219461668386</v>
+      </c>
+      <c r="J601" t="n">
+        <v>0.540372168283071</v>
+      </c>
+      <c r="K601" t="n">
+        <v>0.6471241394625805</v>
+      </c>
+      <c r="L601" t="n">
+        <v>0.7848628823872634</v>
+      </c>
     </row>
     <row r="602">
       <c r="A602" t="s">
@@ -19661,11 +19721,21 @@
       <c r="G603" t="n">
         <v>0.0</v>
       </c>
-      <c r="H603"/>
-      <c r="I603"/>
-      <c r="J603"/>
-      <c r="K603"/>
-      <c r="L603"/>
+      <c r="H603" t="n">
+        <v>0.3823497878761381</v>
+      </c>
+      <c r="I603" t="n">
+        <v>0.32309551718907115</v>
+      </c>
+      <c r="J603" t="n">
+        <v>0.9123407056321989</v>
+      </c>
+      <c r="K603" t="n">
+        <v>0.9706896551724138</v>
+      </c>
+      <c r="L603" t="n">
+        <v>0.7263819095477387</v>
+      </c>
     </row>
     <row r="604">
       <c r="A604" t="s">
@@ -19689,11 +19759,21 @@
       <c r="G604" t="n">
         <v>0.0</v>
       </c>
-      <c r="H604"/>
-      <c r="I604"/>
-      <c r="J604"/>
-      <c r="K604"/>
-      <c r="L604"/>
+      <c r="H604" t="n">
+        <v>0.3904948922600501</v>
+      </c>
+      <c r="I604" t="n">
+        <v>0.32857834549222686</v>
+      </c>
+      <c r="J604" t="n">
+        <v>0.9104111829870422</v>
+      </c>
+      <c r="K604" t="n">
+        <v>0.9730639730639731</v>
+      </c>
+      <c r="L604" t="n">
+        <v>0.7270841192003018</v>
+      </c>
     </row>
     <row r="605">
       <c r="A605" t="s">
@@ -19745,11 +19825,21 @@
       <c r="G606" t="n">
         <v>0.0</v>
       </c>
-      <c r="H606"/>
-      <c r="I606"/>
-      <c r="J606"/>
-      <c r="K606"/>
-      <c r="L606"/>
+      <c r="H606" t="n">
+        <v>0.5021747692515613</v>
+      </c>
+      <c r="I606" t="n">
+        <v>0.41466692112629105</v>
+      </c>
+      <c r="J606" t="n">
+        <v>0.8844243231580867</v>
+      </c>
+      <c r="K606" t="n">
+        <v>0.9351851851851852</v>
+      </c>
+      <c r="L606" t="n">
+        <v>0.7324695121951219</v>
+      </c>
     </row>
     <row r="607">
       <c r="A607" t="s">
@@ -19773,11 +19863,21 @@
       <c r="G607" t="n">
         <v>0.0</v>
       </c>
-      <c r="H607"/>
-      <c r="I607"/>
-      <c r="J607"/>
-      <c r="K607"/>
-      <c r="L607"/>
+      <c r="H607" t="n">
+        <v>0.5130073192020291</v>
+      </c>
+      <c r="I607" t="n">
+        <v>0.4230734575625273</v>
+      </c>
+      <c r="J607" t="n">
+        <v>0.8807567888857353</v>
+      </c>
+      <c r="K607" t="n">
+        <v>0.9355246523388117</v>
+      </c>
+      <c r="L607" t="n">
+        <v>0.7339741549430263</v>
+      </c>
     </row>
     <row r="608">
       <c r="A608" t="s">
@@ -19829,11 +19929,21 @@
       <c r="G609" t="n">
         <v>0.0</v>
       </c>
-      <c r="H609"/>
-      <c r="I609"/>
-      <c r="J609"/>
-      <c r="K609"/>
-      <c r="L609"/>
+      <c r="H609" t="n">
+        <v>0.525131509760614</v>
+      </c>
+      <c r="I609" t="n">
+        <v>0.42026752851169413</v>
+      </c>
+      <c r="J609" t="n">
+        <v>0.5861423656810953</v>
+      </c>
+      <c r="K609" t="n">
+        <v>0.71001221001221</v>
+      </c>
+      <c r="L609" t="n">
+        <v>0.8039171203871749</v>
+      </c>
     </row>
     <row r="610">
       <c r="A610" t="s">
@@ -19857,11 +19967,21 @@
       <c r="G610" t="n">
         <v>0.0</v>
       </c>
-      <c r="H610"/>
-      <c r="I610"/>
-      <c r="J610"/>
-      <c r="K610"/>
-      <c r="L610"/>
+      <c r="H610" t="n">
+        <v>0.48990977323459933</v>
+      </c>
+      <c r="I610" t="n">
+        <v>0.3906029489080301</v>
+      </c>
+      <c r="J610" t="n">
+        <v>0.540372168283071</v>
+      </c>
+      <c r="K610" t="n">
+        <v>0.6867369589345172</v>
+      </c>
+      <c r="L610" t="n">
+        <v>0.8104838709677419</v>
+      </c>
     </row>
     <row r="611">
       <c r="A611" t="s">
@@ -19913,11 +20033,21 @@
       <c r="G612" t="n">
         <v>0.0</v>
       </c>
-      <c r="H612"/>
-      <c r="I612"/>
-      <c r="J612"/>
-      <c r="K612"/>
-      <c r="L612"/>
+      <c r="H612" t="n">
+        <v>0.38455415334605153</v>
+      </c>
+      <c r="I612" t="n">
+        <v>0.3246303998019212</v>
+      </c>
+      <c r="J612" t="n">
+        <v>0.9123407056321989</v>
+      </c>
+      <c r="K612" t="n">
+        <v>0.9705882352941176</v>
+      </c>
+      <c r="L612" t="n">
+        <v>0.7518527823137797</v>
+      </c>
     </row>
     <row r="613">
       <c r="A613" t="s">
@@ -19941,11 +20071,21 @@
       <c r="G613" t="n">
         <v>0.0</v>
       </c>
-      <c r="H613"/>
-      <c r="I613"/>
-      <c r="J613"/>
-      <c r="K613"/>
-      <c r="L613"/>
+      <c r="H613" t="n">
+        <v>0.3927782330341543</v>
+      </c>
+      <c r="I613" t="n">
+        <v>0.3301422006966366</v>
+      </c>
+      <c r="J613" t="n">
+        <v>0.9104111829870422</v>
+      </c>
+      <c r="K613" t="n">
+        <v>0.9713322091062394</v>
+      </c>
+      <c r="L613" t="n">
+        <v>0.752561765260577</v>
+      </c>
     </row>
     <row r="614">
       <c r="A614" t="s">
@@ -19997,11 +20137,21 @@
       <c r="G615" t="n">
         <v>0.0</v>
       </c>
-      <c r="H615"/>
-      <c r="I615"/>
-      <c r="J615"/>
-      <c r="K615"/>
-      <c r="L615"/>
+      <c r="H615" t="n">
+        <v>0.5052850907873817</v>
+      </c>
+      <c r="I615" t="n">
+        <v>0.4166629113791644</v>
+      </c>
+      <c r="J615" t="n">
+        <v>0.8844243231580867</v>
+      </c>
+      <c r="K615" t="n">
+        <v>0.9463806970509383</v>
+      </c>
+      <c r="L615" t="n">
+        <v>0.7584105623968516</v>
+      </c>
     </row>
     <row r="616">
       <c r="A616" t="s">
@@ -20025,11 +20175,21 @@
       <c r="G616" t="n">
         <v>0.0</v>
       </c>
-      <c r="H616"/>
-      <c r="I616"/>
-      <c r="J616"/>
-      <c r="K616"/>
-      <c r="L616"/>
+      <c r="H616" t="n">
+        <v>0.5162045949918995</v>
+      </c>
+      <c r="I616" t="n">
+        <v>0.4251111185434582</v>
+      </c>
+      <c r="J616" t="n">
+        <v>0.8807567888857353</v>
+      </c>
+      <c r="K616" t="n">
+        <v>0.9427083333333334</v>
+      </c>
+      <c r="L616" t="n">
+        <v>0.7592168827866769</v>
+      </c>
     </row>
     <row r="617">
       <c r="A617" t="s">
@@ -20081,11 +20241,21 @@
       <c r="G618" t="n">
         <v>0.0</v>
       </c>
-      <c r="H618"/>
-      <c r="I618"/>
-      <c r="J618"/>
-      <c r="K618"/>
-      <c r="L618"/>
+      <c r="H618" t="n">
+        <v>0.528934320729364</v>
+      </c>
+      <c r="I618" t="n">
+        <v>0.4223176577092402</v>
+      </c>
+      <c r="J618" t="n">
+        <v>0.5861423656810953</v>
+      </c>
+      <c r="K618" t="n">
+        <v>0.7399527186761229</v>
+      </c>
+      <c r="L618" t="n">
+        <v>0.8285693182657508</v>
+      </c>
     </row>
     <row r="619">
       <c r="A619" t="s">
@@ -20109,11 +20279,21 @@
       <c r="G619" t="n">
         <v>0.0</v>
       </c>
-      <c r="H619"/>
-      <c r="I619"/>
-      <c r="J619"/>
-      <c r="K619"/>
-      <c r="L619"/>
+      <c r="H619" t="n">
+        <v>0.49350130809930975</v>
+      </c>
+      <c r="I619" t="n">
+        <v>0.3925141653334392</v>
+      </c>
+      <c r="J619" t="n">
+        <v>0.540372168283071</v>
+      </c>
+      <c r="K619" t="n">
+        <v>0.7238154613466334</v>
+      </c>
+      <c r="L619" t="n">
+        <v>0.8352392416491122</v>
+      </c>
     </row>
     <row r="620">
       <c r="A620" t="s">
@@ -20165,11 +20345,21 @@
       <c r="G621" t="n">
         <v>0.0</v>
       </c>
-      <c r="H621"/>
-      <c r="I621"/>
-      <c r="J621"/>
-      <c r="K621"/>
-      <c r="L621"/>
+      <c r="H621" t="n">
+        <v>0.3929579321024846</v>
+      </c>
+      <c r="I621" t="n">
+        <v>0.3276180797338138</v>
+      </c>
+      <c r="J621" t="n">
+        <v>0.9123407056321989</v>
+      </c>
+      <c r="K621" t="n">
+        <v>0.9633401221995926</v>
+      </c>
+      <c r="L621" t="n">
+        <v>0.7953026422637266</v>
+      </c>
     </row>
     <row r="622">
       <c r="A622" t="s">
@@ -20193,11 +20383,21 @@
       <c r="G622" t="n">
         <v>0.0</v>
       </c>
-      <c r="H622"/>
-      <c r="I622"/>
-      <c r="J622"/>
-      <c r="K622"/>
-      <c r="L622"/>
+      <c r="H622" t="n">
+        <v>0.39081888883338844</v>
+      </c>
+      <c r="I622" t="n">
+        <v>0.3255608810195392</v>
+      </c>
+      <c r="J622" t="n">
+        <v>0.9248920645898275</v>
+      </c>
+      <c r="K622" t="n">
+        <v>0.9638095238095238</v>
+      </c>
+      <c r="L622" t="n">
+        <v>0.7969327073552426</v>
+      </c>
     </row>
     <row r="623">
       <c r="A623" t="s">
@@ -20249,11 +20449,21 @@
       <c r="G624" t="n">
         <v>0.0</v>
       </c>
-      <c r="H624"/>
-      <c r="I624"/>
-      <c r="J624"/>
-      <c r="K624"/>
-      <c r="L624"/>
+      <c r="H624" t="n">
+        <v>0.5167676068138207</v>
+      </c>
+      <c r="I624" t="n">
+        <v>0.4205829469392376</v>
+      </c>
+      <c r="J624" t="n">
+        <v>0.8844243231580867</v>
+      </c>
+      <c r="K624" t="n">
+        <v>0.9451303155006858</v>
+      </c>
+      <c r="L624" t="n">
+        <v>0.8059095808762919</v>
+      </c>
     </row>
     <row r="625">
       <c r="A625" t="s">
@@ -20277,11 +20487,21 @@
       <c r="G625" t="n">
         <v>0.0</v>
       </c>
-      <c r="H625"/>
-      <c r="I625"/>
-      <c r="J625"/>
-      <c r="K625"/>
-      <c r="L625"/>
+      <c r="H625" t="n">
+        <v>0.5179632945197977</v>
+      </c>
+      <c r="I625" t="n">
+        <v>0.4223774590907704</v>
+      </c>
+      <c r="J625" t="n">
+        <v>0.8819629755320219</v>
+      </c>
+      <c r="K625" t="n">
+        <v>0.9407894736842105</v>
+      </c>
+      <c r="L625" t="n">
+        <v>0.8071791613722998</v>
+      </c>
     </row>
     <row r="626">
       <c r="A626" t="s">
@@ -20333,11 +20553,21 @@
       <c r="G627" t="n">
         <v>0.0</v>
       </c>
-      <c r="H627"/>
-      <c r="I627"/>
-      <c r="J627"/>
-      <c r="K627"/>
-      <c r="L627"/>
+      <c r="H627" t="n">
+        <v>0.5418602944533498</v>
+      </c>
+      <c r="I627" t="n">
+        <v>0.4263936675085872</v>
+      </c>
+      <c r="J627" t="n">
+        <v>0.5861423656810953</v>
+      </c>
+      <c r="K627" t="n">
+        <v>0.7674810446503791</v>
+      </c>
+      <c r="L627" t="n">
+        <v>0.8635140874982302</v>
+      </c>
     </row>
     <row r="628">
       <c r="A628" t="s">
@@ -20361,11 +20591,21 @@
       <c r="G628" t="n">
         <v>0.0</v>
       </c>
-      <c r="H628"/>
-      <c r="I628"/>
-      <c r="J628"/>
-      <c r="K628"/>
-      <c r="L628"/>
+      <c r="H628" t="n">
+        <v>0.5438910092497575</v>
+      </c>
+      <c r="I628" t="n">
+        <v>0.4281347906443249</v>
+      </c>
+      <c r="J628" t="n">
+        <v>0.5878746147889197</v>
+      </c>
+      <c r="K628" t="n">
+        <v>0.7302816901408451</v>
+      </c>
+      <c r="L628" t="n">
+        <v>0.8773060029282577</v>
+      </c>
     </row>
     <row r="629">
       <c r="A629" t="s">
@@ -20417,11 +20657,21 @@
       <c r="G630" t="n">
         <v>0.0</v>
       </c>
-      <c r="H630"/>
-      <c r="I630"/>
-      <c r="J630"/>
-      <c r="K630"/>
-      <c r="L630"/>
+      <c r="H630" t="n">
+        <v>0.43445002942996563</v>
+      </c>
+      <c r="I630" t="n">
+        <v>0.30741873339957565</v>
+      </c>
+      <c r="J630" t="n">
+        <v>0.828018210055704</v>
+      </c>
+      <c r="K630" t="n">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="L630" t="n">
+        <v>0.8842406876790831</v>
+      </c>
     </row>
     <row r="631">
       <c r="A631" t="s">
@@ -20445,11 +20695,21 @@
       <c r="G631" t="n">
         <v>0.0</v>
       </c>
-      <c r="H631"/>
-      <c r="I631"/>
-      <c r="J631"/>
-      <c r="K631"/>
-      <c r="L631"/>
+      <c r="H631" t="n">
+        <v>0.446704531147796</v>
+      </c>
+      <c r="I631" t="n">
+        <v>0.3125357315394587</v>
+      </c>
+      <c r="J631" t="n">
+        <v>0.8308291261911909</v>
+      </c>
+      <c r="K631" t="n">
+        <v>0.8894472361809045</v>
+      </c>
+      <c r="L631" t="n">
+        <v>0.8892520669102095</v>
+      </c>
     </row>
     <row r="632">
       <c r="A632" t="s">
@@ -20501,11 +20761,21 @@
       <c r="G633" t="n">
         <v>0.0</v>
       </c>
-      <c r="H633"/>
-      <c r="I633"/>
-      <c r="J633"/>
-      <c r="K633"/>
-      <c r="L633"/>
+      <c r="H633" t="n">
+        <v>0.5117645949022204</v>
+      </c>
+      <c r="I633" t="n">
+        <v>0.3522441977400258</v>
+      </c>
+      <c r="J633" t="n">
+        <v>0.733045202648451</v>
+      </c>
+      <c r="K633" t="n">
+        <v>0.8389513108614233</v>
+      </c>
+      <c r="L633" t="n">
+        <v>0.8969413598285603</v>
+      </c>
     </row>
     <row r="634">
       <c r="A634" t="s">
@@ -20529,11 +20799,21 @@
       <c r="G634" t="n">
         <v>0.0</v>
       </c>
-      <c r="H634"/>
-      <c r="I634"/>
-      <c r="J634"/>
-      <c r="K634"/>
-      <c r="L634"/>
+      <c r="H634" t="n">
+        <v>0.5168421340123284</v>
+      </c>
+      <c r="I634" t="n">
+        <v>0.35383897393016095</v>
+      </c>
+      <c r="J634" t="n">
+        <v>0.7290896809931678</v>
+      </c>
+      <c r="K634" t="n">
+        <v>0.8303249097472925</v>
+      </c>
+      <c r="L634" t="n">
+        <v>0.8979113800507516</v>
+      </c>
     </row>
     <row r="635">
       <c r="A635" t="s">
@@ -20585,11 +20865,21 @@
       <c r="G636" t="n">
         <v>0.0</v>
       </c>
-      <c r="H636"/>
-      <c r="I636"/>
-      <c r="J636"/>
-      <c r="K636"/>
-      <c r="L636"/>
+      <c r="H636" t="n">
+        <v>0.43160108295277955</v>
+      </c>
+      <c r="I636" t="n">
+        <v>0.29063396977968703</v>
+      </c>
+      <c r="J636" t="n">
+        <v>0.5280575399523143</v>
+      </c>
+      <c r="K636" t="n">
+        <v>0.5951972555746141</v>
+      </c>
+      <c r="L636" t="n">
+        <v>0.9157151754203862</v>
+      </c>
     </row>
     <row r="637">
       <c r="A637" t="s">
@@ -20613,11 +20903,21 @@
       <c r="G637" t="n">
         <v>0.0</v>
       </c>
-      <c r="H637"/>
-      <c r="I637"/>
-      <c r="J637"/>
-      <c r="K637"/>
-      <c r="L637"/>
+      <c r="H637" t="n">
+        <v>0.4134759627671508</v>
+      </c>
+      <c r="I637" t="n">
+        <v>0.2769494821753848</v>
+      </c>
+      <c r="J637" t="n">
+        <v>0.5081153680062789</v>
+      </c>
+      <c r="K637" t="n">
+        <v>0.5681470137825421</v>
+      </c>
+      <c r="L637" t="n">
+        <v>0.9195281230250685</v>
+      </c>
     </row>
     <row r="638">
       <c r="A638" t="s">
@@ -20669,11 +20969,21 @@
       <c r="G639" t="n">
         <v>0.0</v>
       </c>
-      <c r="H639"/>
-      <c r="I639"/>
-      <c r="J639"/>
-      <c r="K639"/>
-      <c r="L639"/>
+      <c r="H639" t="n">
+        <v>0.43785391520307454</v>
+      </c>
+      <c r="I639" t="n">
+        <v>0.30889502730964874</v>
+      </c>
+      <c r="J639" t="n">
+        <v>0.828018210055704</v>
+      </c>
+      <c r="K639" t="n">
+        <v>0.8848484848484849</v>
+      </c>
+      <c r="L639" t="n">
+        <v>0.897803247373448</v>
+      </c>
     </row>
     <row r="640">
       <c r="A640" t="s">
@@ -20697,11 +21007,21 @@
       <c r="G640" t="n">
         <v>0.0</v>
       </c>
-      <c r="H640"/>
-      <c r="I640"/>
-      <c r="J640"/>
-      <c r="K640"/>
-      <c r="L640"/>
+      <c r="H640" t="n">
+        <v>0.4503908164834533</v>
+      </c>
+      <c r="I640" t="n">
+        <v>0.3140403711042752</v>
+      </c>
+      <c r="J640" t="n">
+        <v>0.8308291261911909</v>
+      </c>
+      <c r="K640" t="n">
+        <v>0.8882978723404256</v>
+      </c>
+      <c r="L640" t="n">
+        <v>0.9013814274750576</v>
+      </c>
     </row>
     <row r="641">
       <c r="A641" t="s">
@@ -20753,11 +21073,21 @@
       <c r="G642" t="n">
         <v>0.0</v>
       </c>
-      <c r="H642"/>
-      <c r="I642"/>
-      <c r="J642"/>
-      <c r="K642"/>
-      <c r="L642"/>
+      <c r="H642" t="n">
+        <v>0.5162265243855738</v>
+      </c>
+      <c r="I642" t="n">
+        <v>0.3539531736819643</v>
+      </c>
+      <c r="J642" t="n">
+        <v>0.733045202648451</v>
+      </c>
+      <c r="K642" t="n">
+        <v>0.8345864661654135</v>
+      </c>
+      <c r="L642" t="n">
+        <v>0.9105960264900662</v>
+      </c>
     </row>
     <row r="643">
       <c r="A643" t="s">
@@ -20781,11 +21111,21 @@
       <c r="G643" t="n">
         <v>0.0</v>
       </c>
-      <c r="H643"/>
-      <c r="I643"/>
-      <c r="J643"/>
-      <c r="K643"/>
-      <c r="L643"/>
+      <c r="H643" t="n">
+        <v>0.5214534842747636</v>
+      </c>
+      <c r="I643" t="n">
+        <v>0.355558188471215</v>
+      </c>
+      <c r="J643" t="n">
+        <v>0.7290896809931678</v>
+      </c>
+      <c r="K643" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="L643" t="n">
+        <v>0.9105058365758755</v>
+      </c>
     </row>
     <row r="644">
       <c r="A644" t="s">
@@ -20837,11 +21177,21 @@
       <c r="G645" t="n">
         <v>0.0</v>
       </c>
-      <c r="H645"/>
-      <c r="I645"/>
-      <c r="J645"/>
-      <c r="K645"/>
-      <c r="L645"/>
+      <c r="H645" t="n">
+        <v>0.4356066086437315</v>
+      </c>
+      <c r="I645" t="n">
+        <v>0.2920400533087781</v>
+      </c>
+      <c r="J645" t="n">
+        <v>0.5280575399523143</v>
+      </c>
+      <c r="K645" t="n">
+        <v>0.6203007518796992</v>
+      </c>
+      <c r="L645" t="n">
+        <v>0.9278964667214462</v>
+      </c>
     </row>
     <row r="646">
       <c r="A646" t="s">
@@ -20865,11 +21215,21 @@
       <c r="G646" t="n">
         <v>0.0</v>
       </c>
-      <c r="H646"/>
-      <c r="I646"/>
-      <c r="J646"/>
-      <c r="K646"/>
-      <c r="L646"/>
+      <c r="H646" t="n">
+        <v>0.4173819763979137</v>
+      </c>
+      <c r="I646" t="n">
+        <v>0.2782908341552996</v>
+      </c>
+      <c r="J646" t="n">
+        <v>0.5081153680062789</v>
+      </c>
+      <c r="K646" t="n">
+        <v>0.5971731448763251</v>
+      </c>
+      <c r="L646" t="n">
+        <v>0.9290442697558957</v>
+      </c>
     </row>
     <row r="647">
       <c r="A647" t="s">
@@ -20921,11 +21281,21 @@
       <c r="G648" t="n">
         <v>0.0</v>
       </c>
-      <c r="H648"/>
-      <c r="I648"/>
-      <c r="J648"/>
-      <c r="K648"/>
-      <c r="L648"/>
+      <c r="H648" t="n">
+        <v>0.454892789255641</v>
+      </c>
+      <c r="I648" t="n">
+        <v>0.31036909929810197</v>
+      </c>
+      <c r="J648" t="n">
+        <v>0.828018210055704</v>
+      </c>
+      <c r="K648" t="n">
+        <v>0.8848484848484849</v>
+      </c>
+      <c r="L648" t="n">
+        <v>0.9021967526265521</v>
+      </c>
     </row>
     <row r="649">
       <c r="A649" t="s">
@@ -20949,11 +21319,21 @@
       <c r="G649" t="n">
         <v>0.0</v>
       </c>
-      <c r="H649"/>
-      <c r="I649"/>
-      <c r="J649"/>
-      <c r="K649"/>
-      <c r="L649"/>
+      <c r="H649" t="n">
+        <v>0.4681372043233213</v>
+      </c>
+      <c r="I649" t="n">
+        <v>0.3155437486279438</v>
+      </c>
+      <c r="J649" t="n">
+        <v>0.8308291261911909</v>
+      </c>
+      <c r="K649" t="n">
+        <v>0.88268156424581</v>
+      </c>
+      <c r="L649" t="n">
+        <v>0.9042329055736449</v>
+      </c>
     </row>
     <row r="650">
       <c r="A650" t="s">
@@ -21005,11 +21385,21 @@
       <c r="G651" t="n">
         <v>0.0</v>
       </c>
-      <c r="H651"/>
-      <c r="I651"/>
-      <c r="J651"/>
-      <c r="K651"/>
-      <c r="L651"/>
+      <c r="H651" t="n">
+        <v>0.5368380738132266</v>
+      </c>
+      <c r="I651" t="n">
+        <v>0.3556543493117752</v>
+      </c>
+      <c r="J651" t="n">
+        <v>0.733045202648451</v>
+      </c>
+      <c r="K651" t="n">
+        <v>0.8435114503816794</v>
+      </c>
+      <c r="L651" t="n">
+        <v>0.9149474503697937</v>
+      </c>
     </row>
     <row r="652">
       <c r="A652" t="s">
@@ -21033,11 +21423,21 @@
       <c r="G652" t="n">
         <v>0.0</v>
       </c>
-      <c r="H652"/>
-      <c r="I652"/>
-      <c r="J652"/>
-      <c r="K652"/>
-      <c r="L652"/>
+      <c r="H652" t="n">
+        <v>0.5423956433481129</v>
+      </c>
+      <c r="I652" t="n">
+        <v>0.3572692590664213</v>
+      </c>
+      <c r="J652" t="n">
+        <v>0.7290896809931678</v>
+      </c>
+      <c r="K652" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="L652" t="n">
+        <v>0.9149805447470817</v>
+      </c>
     </row>
     <row r="653">
       <c r="A653" t="s">
@@ -21089,11 +21489,21 @@
       <c r="G654" t="n">
         <v>0.0</v>
       </c>
-      <c r="H654"/>
-      <c r="I654"/>
-      <c r="J654"/>
-      <c r="K654"/>
-      <c r="L654"/>
+      <c r="H654" t="n">
+        <v>0.453299574190362</v>
+      </c>
+      <c r="I654" t="n">
+        <v>0.29344521206585483</v>
+      </c>
+      <c r="J654" t="n">
+        <v>0.5280575399523143</v>
+      </c>
+      <c r="K654" t="n">
+        <v>0.642570281124498</v>
+      </c>
+      <c r="L654" t="n">
+        <v>0.9310485516115871</v>
+      </c>
     </row>
     <row r="655">
       <c r="A655" t="s">
@@ -21117,11 +21527,21 @@
       <c r="G655" t="n">
         <v>0.0</v>
       </c>
-      <c r="H655"/>
-      <c r="I655"/>
-      <c r="J655"/>
-      <c r="K655"/>
-      <c r="L655"/>
+      <c r="H655" t="n">
+        <v>0.4344188358897779</v>
+      </c>
+      <c r="I655" t="n">
+        <v>0.2796335746330619</v>
+      </c>
+      <c r="J655" t="n">
+        <v>0.5081153680062789</v>
+      </c>
+      <c r="K655" t="n">
+        <v>0.6182495344506518</v>
+      </c>
+      <c r="L655" t="n">
+        <v>0.9329631914456097</v>
+      </c>
     </row>
     <row r="656">
       <c r="A656" t="s">
@@ -21173,11 +21593,21 @@
       <c r="G657" t="n">
         <v>0.0</v>
       </c>
-      <c r="H657"/>
-      <c r="I657"/>
-      <c r="J657"/>
-      <c r="K657"/>
-      <c r="L657"/>
+      <c r="H657" t="n">
+        <v>0.46175600473454226</v>
+      </c>
+      <c r="I657" t="n">
+        <v>0.31327337239877606</v>
+      </c>
+      <c r="J657" t="n">
+        <v>0.828018210055704</v>
+      </c>
+      <c r="K657" t="n">
+        <v>0.8867924528301887</v>
+      </c>
+      <c r="L657" t="n">
+        <v>0.9149017363098645</v>
+      </c>
     </row>
     <row r="658">
       <c r="A658" t="s">
@@ -21201,11 +21631,21 @@
       <c r="G658" t="n">
         <v>0.0</v>
       </c>
-      <c r="H658"/>
-      <c r="I658"/>
-      <c r="J658"/>
-      <c r="K658"/>
-      <c r="L658"/>
+      <c r="H658" t="n">
+        <v>0.46027963150212203</v>
+      </c>
+      <c r="I658" t="n">
+        <v>0.31237545163086405</v>
+      </c>
+      <c r="J658" t="n">
+        <v>0.8281075015977591</v>
+      </c>
+      <c r="K658" t="n">
+        <v>0.8881987577639752</v>
+      </c>
+      <c r="L658" t="n">
+        <v>0.9152510020996374</v>
+      </c>
     </row>
     <row r="659">
       <c r="A659" t="s">
@@ -21257,11 +21697,21 @@
       <c r="G660" t="n">
         <v>0.0</v>
       </c>
-      <c r="H660"/>
-      <c r="I660"/>
-      <c r="J660"/>
-      <c r="K660"/>
-      <c r="L660"/>
+      <c r="H660" t="n">
+        <v>0.5459411712078307</v>
+      </c>
+      <c r="I660" t="n">
+        <v>0.3590445874609075</v>
+      </c>
+      <c r="J660" t="n">
+        <v>0.733045202648451</v>
+      </c>
+      <c r="K660" t="n">
+        <v>0.848605577689243</v>
+      </c>
+      <c r="L660" t="n">
+        <v>0.9273645368032628</v>
+      </c>
     </row>
     <row r="661">
       <c r="A661" t="s">
@@ -21285,11 +21735,21 @@
       <c r="G661" t="n">
         <v>0.0</v>
       </c>
-      <c r="H661"/>
-      <c r="I661"/>
-      <c r="J661"/>
-      <c r="K661"/>
-      <c r="L661"/>
+      <c r="H661" t="n">
+        <v>0.5431879160883067</v>
+      </c>
+      <c r="I661" t="n">
+        <v>0.35749843186536034</v>
+      </c>
+      <c r="J661" t="n">
+        <v>0.7265112051562631</v>
+      </c>
+      <c r="K661" t="n">
+        <v>0.8443579766536965</v>
+      </c>
+      <c r="L661" t="n">
+        <v>0.9280575539568345</v>
+      </c>
     </row>
     <row r="662">
       <c r="A662" t="s">
@@ -21341,11 +21801,21 @@
       <c r="G663" t="n">
         <v>0.0</v>
       </c>
-      <c r="H663"/>
-      <c r="I663"/>
-      <c r="J663"/>
-      <c r="K663"/>
-      <c r="L663"/>
+      <c r="H663" t="n">
+        <v>0.461540377220559</v>
+      </c>
+      <c r="I663" t="n">
+        <v>0.2962473185622385</v>
+      </c>
+      <c r="J663" t="n">
+        <v>0.5280575399523143</v>
+      </c>
+      <c r="K663" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="L663" t="n">
+        <v>0.9366</v>
+      </c>
     </row>
     <row r="664">
       <c r="A664" t="s">
@@ -21369,11 +21839,21 @@
       <c r="G664" t="n">
         <v>0.0</v>
       </c>
-      <c r="H664"/>
-      <c r="I664"/>
-      <c r="J664"/>
-      <c r="K664"/>
-      <c r="L664"/>
+      <c r="H664" t="n">
+        <v>0.461540377220559</v>
+      </c>
+      <c r="I664" t="n">
+        <v>0.2962473185622385</v>
+      </c>
+      <c r="J664" t="n">
+        <v>0.5280575399523143</v>
+      </c>
+      <c r="K664" t="n">
+        <v>0.627906976744186</v>
+      </c>
+      <c r="L664" t="n">
+        <v>0.941140653541709</v>
+      </c>
     </row>
     <row r="665">
       <c r="A665" t="s">

</xml_diff>